<commit_message>
Emilie's code and data
</commit_message>
<xml_diff>
--- a/finalsubmissiondata/issuers.xlsx
+++ b/finalsubmissiondata/issuers.xlsx
@@ -55,7 +55,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -439,15 +438,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:G1036"/>
+  <dimension ref="A1:I1036"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="G172" sqref="G172"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>349570</v>
       </c>
@@ -495,8 +494,12 @@
         <f>E2+F2</f>
         <v>28.699163275553421</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2">
+        <f>65*B2</f>
+        <v>516620</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>351274</v>
       </c>
@@ -510,7 +513,7 @@
         <v>46.700680272108798</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>353486</v>
       </c>
@@ -524,7 +527,7 @@
         <v>46.389610389610297</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>346105</v>
       </c>
@@ -538,7 +541,7 @@
         <v>46.208860759493597</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>356304</v>
       </c>
@@ -552,7 +555,7 @@
         <v>44.3197674418604</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>347489</v>
       </c>
@@ -566,7 +569,7 @@
         <v>44.305699481865197</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>347687</v>
       </c>
@@ -580,7 +583,7 @@
         <v>43.6196319018404</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>358194</v>
       </c>
@@ -594,7 +597,7 @@
         <v>43.5416666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>355134</v>
       </c>
@@ -608,7 +611,7 @@
         <v>43.076923076923002</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>357792</v>
       </c>
@@ -622,7 +625,7 @@
         <v>42.337278106508798</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>358623</v>
       </c>
@@ -636,7 +639,7 @@
         <v>41.338235294117602</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>349481</v>
       </c>
@@ -650,7 +653,7 @@
         <v>41.205673758865203</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>357783</v>
       </c>
@@ -664,7 +667,7 @@
         <v>40.308510638297797</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>357360</v>
       </c>
@@ -678,7 +681,7 @@
         <v>40.2625698324022</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>354098</v>
       </c>
@@ -14968,7 +14971,6 @@
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>